<commit_message>
Update with the files from week 3
</commit_message>
<xml_diff>
--- a/RiskRegister.xlsx
+++ b/RiskRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thwai\Desktop\Ecen 3753\Final Project\RTOS_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13113F5-B79F-4AB1-BC2B-2EE0490D5BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E170C43E-69F1-4B46-890E-61D7BE3DCD58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>I get overloaded with work from my capstone</t>
   </si>
   <si>
-    <t>Work Ahead to account for one week of lost time</t>
-  </si>
-  <si>
     <t>Do no update until after the project is finished</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>know the instructor has extension and ask if sick, also getting vaccine</t>
+  </si>
+  <si>
+    <t>Work Ahead to account for one week of lost time, finished my capstone techical work</t>
   </si>
 </sst>
 </file>
@@ -317,41 +317,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -359,41 +356,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1282,13 +1276,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>232681</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>146503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>210456</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>127453</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1318,8 +1312,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0" headerRowBorderDxfId="6">
-  <autoFilter ref="A1:H13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowBorderDxfId="6">
+  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="P" dataDxfId="5"/>
@@ -1612,7 +1606,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1624,7 +1618,7 @@
     <col min="5" max="5" width="12.15234375" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.53515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.15234375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="60.53515625" customWidth="1"/>
+    <col min="8" max="8" width="74.23046875" customWidth="1"/>
     <col min="9" max="9" width="36.3046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1658,7 +1652,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1">
         <v>20</v>
@@ -1680,61 +1674,59 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
         <v>20</v>
       </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D9" si="1">B3*C3</f>
-        <v>260</v>
+        <f>B3*C3</f>
+        <v>160</v>
       </c>
       <c r="E3" s="2">
         <v>44287</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <f>B4*C4</f>
+        <v>100</v>
       </c>
       <c r="E4" s="2">
         <v>44287</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -1748,81 +1740,81 @@
         <v>40</v>
       </c>
       <c r="D5" s="1">
+        <f t="shared" ref="D5:D8" si="1">B5*C5</f>
+        <v>80</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44295</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="E5" s="2">
-        <v>44295</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>100</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
       <c r="E6" s="2">
         <v>44287</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2">
         <v>44287</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
         <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
@@ -1833,117 +1825,119 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>20</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" ref="D9" si="2">B9*C9</f>
+        <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>44287</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" ref="D10" si="2">B10*C10</f>
+        <f>B10*C10</f>
         <v>40</v>
       </c>
       <c r="E10" s="2">
         <v>44287</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
         <v>29</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
         <f>B11*C11</f>
         <v>40</v>
       </c>
       <c r="E11" s="2">
-        <v>44287</v>
+        <v>44295</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <f>B12*C12</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2">
-        <v>44295</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>44302</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J11">
-    <sortCondition descending="1" ref="D5:D11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J10">
+    <sortCondition descending="1" ref="D5:D10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1958,7 +1952,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C12 C13</xm:sqref>
+          <xm:sqref>B2:C5 B6:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Update to include needed report
</commit_message>
<xml_diff>
--- a/RiskRegister.xlsx
+++ b/RiskRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thwai\Desktop\Ecen 3753\Final Project\RTOS_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E170C43E-69F1-4B46-890E-61D7BE3DCD58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C077DF75-2F99-4D47-8580-B7CC1ABAA874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Item</t>
   </si>
@@ -133,19 +133,22 @@
     <t>The LCD takes too much compute time</t>
   </si>
   <si>
-    <t>Limit Processing of other tasks</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capsense readings are slow </t>
   </si>
   <si>
-    <t>May be somewhat slow but game should still be playable</t>
-  </si>
-  <si>
     <t>know the instructor has extension and ask if sick, also getting vaccine</t>
   </si>
   <si>
     <t>Work Ahead to account for one week of lost time, finished my capstone techical work</t>
+  </si>
+  <si>
+    <t>Resloved</t>
+  </si>
+  <si>
+    <t>LCD is implemented and does not take too much time</t>
+  </si>
+  <si>
+    <t>The Capsense has been implemented with no impact to playability</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.3793054408758727E-2"/>
+          <c:y val="6.4494902980150592E-2"/>
+          <c:w val="0.88614978381258236"/>
+          <c:h val="0.74476922033352355"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -317,78 +330,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1606,7 +1625,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1652,86 +1671,86 @@
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
         <v>20</v>
       </c>
-      <c r="C2" s="1">
-        <v>40</v>
-      </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2" si="0">B2*C2</f>
-        <v>800</v>
+        <f>B2*C2</f>
+        <v>160</v>
       </c>
       <c r="E2" s="2">
-        <v>44295</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>44287</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1">
         <f>B3*C3</f>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2">
         <v>44287</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
-        <f>B4*C4</f>
-        <v>100</v>
+        <f t="shared" ref="D4:D7" si="0">B4*C4</f>
+        <v>80</v>
       </c>
       <c r="E4" s="2">
-        <v>44287</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>44295</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -1740,59 +1759,57 @@
         <v>40</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D8" si="1">B5*C5</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E5" s="2">
-        <v>44295</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>44287</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="E6" s="2">
         <v>44287</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
         <v>20</v>
       </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="E7" s="2">
@@ -1800,133 +1817,137 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>20</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" ref="D8" si="1">B8*C8</f>
+        <v>40</v>
       </c>
       <c r="E8" s="2">
         <v>44287</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9" si="2">B9*C9</f>
+        <f>B9*C9</f>
         <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>44287</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1">
         <f>B10*C10</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2">
-        <v>44287</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>44302</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
         <f>B11*C11</f>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
         <v>44295</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*C12</f>
-        <v>39</v>
+        <f t="shared" ref="D12" si="2">B12*C12</f>
+        <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>44302</v>
+        <v>44307</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>11</v>
@@ -1936,8 +1957,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J10">
-    <sortCondition descending="1" ref="D5:D10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J10">
+    <sortCondition descending="1" ref="D4:D10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1952,7 +1973,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C5 B6:C12</xm:sqref>
+          <xm:sqref>B2:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>